<commit_message>
Adding react-apps and timesheet
React-app, one works, one does not. Both are connected to the contentful environment.
</commit_message>
<xml_diff>
--- a/Admin/Timesheets/Cameron/timesheet(09-26 to 09-30).xlsx
+++ b/Admin/Timesheets/Cameron/timesheet(09-26 to 09-30).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cambo\Documents\GitHub\CongruexTeam\Admin\Timesheets\Cameron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9850CEDF-CDA1-48B8-ACC7-5D4C63DEC640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF185FB8-94BF-46A5-BAA5-3F98AB6A9333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -71,24 +71,6 @@
     <t>Sponsor Meeting</t>
   </si>
   <si>
-    <t>Task aaaaa</t>
-  </si>
-  <si>
-    <t>Task bbbbb</t>
-  </si>
-  <si>
-    <t>Task ccccc</t>
-  </si>
-  <si>
-    <t>Task xxxxxx</t>
-  </si>
-  <si>
-    <t>Task yyyyy</t>
-  </si>
-  <si>
-    <t>Task zzzzzz</t>
-  </si>
-  <si>
     <t>Tasks align with the project plan</t>
   </si>
   <si>
@@ -111,6 +93,12 @@
   </si>
   <si>
     <t>Congruex</t>
+  </si>
+  <si>
+    <t>Research CDS</t>
+  </si>
+  <si>
+    <t>Practice React</t>
   </si>
 </sst>
 </file>
@@ -516,16 +504,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.140625" customWidth="1"/>
   </cols>
@@ -535,7 +526,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -547,10 +538,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -589,25 +580,25 @@
         <v>2</v>
       </c>
       <c r="B5" s="10">
-        <v>42029</v>
+        <v>44830</v>
       </c>
       <c r="C5" s="10">
-        <v>42030</v>
+        <v>44831</v>
       </c>
       <c r="D5" s="10">
-        <v>42031</v>
+        <v>44832</v>
       </c>
       <c r="E5" s="10">
-        <v>42032</v>
+        <v>42033</v>
       </c>
       <c r="F5" s="10">
-        <v>42033</v>
+        <v>44834</v>
       </c>
       <c r="G5" s="10">
-        <v>42034</v>
+        <v>44835</v>
       </c>
       <c r="H5" s="11">
-        <v>42035</v>
+        <v>44836</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>5</v>
@@ -617,7 +608,9 @@
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -625,8 +618,8 @@
       <c r="G6" s="1"/>
       <c r="H6" s="3"/>
       <c r="I6" s="4">
-        <f t="shared" ref="I6:I14" si="0">SUM(B6:H6)</f>
-        <v>0</v>
+        <f t="shared" ref="I6:I11" si="0">SUM(B6:H6)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -649,16 +642,22 @@
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="3"/>
       <c r="I8" s="4">
         <f t="shared" ref="I8" si="1">SUM(B8:H8)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -679,170 +678,134 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
       <c r="I10" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
       <c r="I11" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="3"/>
+      <c r="A12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="4">
+        <f>SUM(B6:B11)</f>
+        <v>4</v>
+      </c>
+      <c r="C12" s="4">
+        <f>SUM(C6:C11)</f>
+        <v>2</v>
+      </c>
+      <c r="D12" s="4">
+        <f>SUM(D6:D11)</f>
+        <v>3</v>
+      </c>
+      <c r="E12" s="4">
+        <f>SUM(E6:E11)</f>
+        <v>2</v>
+      </c>
+      <c r="F12" s="4">
+        <f>SUM(F6:F11)</f>
+        <v>3</v>
+      </c>
+      <c r="G12" s="4">
+        <f>SUM(G6:G11)</f>
+        <v>2</v>
+      </c>
+      <c r="H12" s="4">
+        <f>SUM(H6:H11)</f>
+        <v>2</v>
+      </c>
       <c r="I12" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+        <f>SUM(I6:I11)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="4">
-        <f t="shared" ref="I15" si="2">SUM(B15:H15)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="4">
-        <f>SUM(B6:B15)</f>
-        <v>0</v>
-      </c>
-      <c r="C16" s="4">
-        <f t="shared" ref="C16:H16" si="3">SUM(C6:C15)</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="4">
-        <f>SUM(I6:I15)</f>
-        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>4</v>
+      <c r="A19" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>19</v>
+      <c r="A20" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>